<commit_message>
coef low and high
</commit_message>
<xml_diff>
--- a/A2_results_step1.xlsx
+++ b/A2_results_step1.xlsx
@@ -392,7 +392,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>1.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -417,12 +417,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>0.0</v>
+        <v>10.500000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -437,7 +437,7 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -447,7 +447,7 @@
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>1.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -462,7 +462,7 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -472,7 +472,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -492,7 +492,7 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="23" spans="1:1">

</xml_diff>